<commit_message>
Transformiral vsako tabelo posebej
</commit_message>
<xml_diff>
--- a/podatki/kazalniki_bolniškega_staleža_po_statističnih_regijah_in_spolu.xlsx
+++ b/podatki/kazalniki_bolniškega_staleža_po_statističnih_regijah_in_spolu.xlsx
@@ -20,7 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+  <si>
+    <t xml:space="preserve">Spol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oznaka regije</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tip_podatka</t>
+  </si>
   <si>
     <t xml:space="preserve">2008</t>
   </si>
@@ -346,10 +358,10 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.97"/>
@@ -360,58 +372,70 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>13.1</v>
@@ -455,13 +479,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>16.5</v>
@@ -505,13 +529,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>14.3</v>
@@ -555,13 +579,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>15.7</v>
@@ -605,13 +629,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>14.5</v>
@@ -655,13 +679,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>18.4</v>
@@ -705,13 +729,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>12</v>
@@ -755,13 +779,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>13.8</v>
@@ -805,13 +829,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>11.5</v>
@@ -855,13 +879,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>12.4</v>
@@ -905,13 +929,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>15</v>
@@ -955,13 +979,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>11.2</v>
@@ -1005,13 +1029,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>13.5</v>
@@ -1055,66 +1079,66 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>18.6</v>
@@ -1158,13 +1182,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>21.5</v>
@@ -1208,13 +1232,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>18</v>
@@ -1258,13 +1282,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>21</v>
@@ -1308,13 +1332,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>20</v>
@@ -1358,13 +1382,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>22.8</v>
@@ -1408,13 +1432,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>15.8</v>
@@ -1458,13 +1482,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>19.3</v>
@@ -1508,13 +1532,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>17.8</v>
@@ -1558,13 +1582,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>17.1</v>
@@ -1608,13 +1632,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>23.2</v>
@@ -1658,13 +1682,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>15.5</v>
@@ -1708,13 +1732,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>21.1</v>
@@ -1758,52 +1782,52 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>